<commit_message>
add challenge tour class + enum attribute to tournament
</commit_message>
<xml_diff>
--- a/Docs/Golf/Rating.xlsx
+++ b/Docs/Golf/Rating.xlsx
@@ -198,10 +198,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -552,14 +552,14 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
@@ -680,7 +680,7 @@
       <c r="H7">
         <v>21</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K7">
@@ -1324,6 +1324,7 @@
   <cols>
     <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>